<commit_message>
Ajout "type d'enseignement" et "systèmes" dans les préférences
</commit_message>
<xml_diff>
--- a/src/SSI_Programme-Progression.xlsx
+++ b/src/SSI_Programme-Progression.xlsx
@@ -945,7 +945,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-40C]d\ mmm"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
@@ -987,13 +987,6 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -1061,13 +1054,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="1"/>
       <color theme="0"/>
       <name val="Arial"/>
@@ -1085,13 +1071,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="3" tint="0.39997558519241921"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1719,7 +1698,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1735,118 +1714,118 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1861,22 +1840,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1897,331 +1876,295 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2570,7 +2513,7 @@
       <pane xSplit="8" ySplit="4" topLeftCell="I5" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="R24" sqref="I1:R1048576"/>
       <selection pane="bottomLeft" activeCell="B1" sqref="B1:AL12"/>
-      <selection pane="bottomRight" activeCell="S11" sqref="S11"/>
+      <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12.75"/>
@@ -2597,42 +2540,42 @@
       <c r="N1" s="28"/>
     </row>
     <row r="2" spans="1:18" ht="12.75" customHeight="1">
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
       <c r="H2" s="71"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="104" t="s">
+      <c r="J2" s="130" t="s">
         <v>207</v>
       </c>
-      <c r="K2" s="108" t="s">
+      <c r="K2" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="108"/>
-      <c r="M2" s="109"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="135"/>
       <c r="N2" s="67"/>
-      <c r="O2" s="110" t="s">
+      <c r="O2" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="108"/>
-      <c r="Q2" s="109"/>
+      <c r="P2" s="134"/>
+      <c r="Q2" s="135"/>
       <c r="R2" s="19"/>
     </row>
     <row r="3" spans="1:18" ht="21" customHeight="1">
-      <c r="B3" s="106"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="106"/>
+      <c r="B3" s="132"/>
+      <c r="C3" s="132"/>
+      <c r="D3" s="132"/>
+      <c r="E3" s="132"/>
+      <c r="F3" s="132"/>
+      <c r="G3" s="132"/>
       <c r="H3" s="71"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="105"/>
+      <c r="J3" s="131"/>
       <c r="K3" s="65">
         <v>1</v>
       </c>
@@ -2659,15 +2602,15 @@
       <c r="R3" s="20"/>
     </row>
     <row r="4" spans="1:18" ht="200.25" customHeight="1" thickBot="1">
-      <c r="B4" s="107"/>
-      <c r="C4" s="107"/>
-      <c r="D4" s="107"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="133"/>
+      <c r="D4" s="133"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="133"/>
+      <c r="G4" s="133"/>
       <c r="H4" s="72"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="105"/>
+      <c r="J4" s="131"/>
       <c r="K4" s="66"/>
       <c r="L4" s="57"/>
       <c r="M4" s="58"/>
@@ -2678,16 +2621,16 @@
       <c r="R4" s="20"/>
     </row>
     <row r="5" spans="1:18" s="7" customFormat="1" ht="39" customHeight="1">
-      <c r="A5" s="131" t="s">
+      <c r="A5" s="157" t="s">
         <v>197</v>
       </c>
-      <c r="B5" s="132"/>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="132"/>
-      <c r="F5" s="132"/>
-      <c r="G5" s="132"/>
-      <c r="H5" s="133"/>
+      <c r="B5" s="158"/>
+      <c r="C5" s="158"/>
+      <c r="D5" s="158"/>
+      <c r="E5" s="158"/>
+      <c r="F5" s="158"/>
+      <c r="G5" s="158"/>
+      <c r="H5" s="159"/>
       <c r="I5" s="64"/>
       <c r="J5" s="80" t="s">
         <v>210</v>
@@ -2818,22 +2761,22 @@
     <row r="10" spans="1:18" s="13" customFormat="1" ht="12">
       <c r="A10" s="46"/>
       <c r="B10" s="47"/>
-      <c r="C10" s="111" t="s">
+      <c r="C10" s="137" t="s">
         <v>198</v>
       </c>
-      <c r="D10" s="116" t="s">
+      <c r="D10" s="142" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="113">
+      <c r="F10" s="139">
         <v>0</v>
       </c>
-      <c r="G10" s="118" t="s">
+      <c r="G10" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="134"/>
+      <c r="H10" s="160"/>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
       <c r="K10" s="82"/>
@@ -2848,14 +2791,14 @@
     <row r="11" spans="1:18" s="13" customFormat="1" ht="12">
       <c r="A11" s="46"/>
       <c r="B11" s="47"/>
-      <c r="C11" s="111"/>
-      <c r="D11" s="116"/>
+      <c r="C11" s="137"/>
+      <c r="D11" s="142"/>
       <c r="E11" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="114"/>
-      <c r="G11" s="118"/>
-      <c r="H11" s="135"/>
+      <c r="F11" s="140"/>
+      <c r="G11" s="144"/>
+      <c r="H11" s="161"/>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
       <c r="K11" s="85"/>
@@ -2870,14 +2813,14 @@
     <row r="12" spans="1:18" s="13" customFormat="1" ht="25.5" customHeight="1">
       <c r="A12" s="46"/>
       <c r="B12" s="47"/>
-      <c r="C12" s="111"/>
-      <c r="D12" s="116"/>
+      <c r="C12" s="137"/>
+      <c r="D12" s="142"/>
       <c r="E12" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="114"/>
-      <c r="G12" s="118"/>
-      <c r="H12" s="135"/>
+      <c r="F12" s="140"/>
+      <c r="G12" s="144"/>
+      <c r="H12" s="161"/>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
       <c r="K12" s="85"/>
@@ -2892,14 +2835,14 @@
     <row r="13" spans="1:18" s="13" customFormat="1" ht="24" customHeight="1">
       <c r="A13" s="46"/>
       <c r="B13" s="47"/>
-      <c r="C13" s="111"/>
-      <c r="D13" s="116"/>
+      <c r="C13" s="137"/>
+      <c r="D13" s="142"/>
       <c r="E13" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="114"/>
-      <c r="G13" s="118"/>
-      <c r="H13" s="136"/>
+      <c r="F13" s="140"/>
+      <c r="G13" s="144"/>
+      <c r="H13" s="162"/>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
       <c r="K13" s="85"/>
@@ -2914,18 +2857,18 @@
     <row r="14" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A14" s="29"/>
       <c r="B14" s="30"/>
-      <c r="C14" s="111"/>
+      <c r="C14" s="137"/>
       <c r="D14" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="137" t="s">
+      <c r="E14" s="163" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="114"/>
-      <c r="G14" s="138" t="s">
+      <c r="F14" s="140"/>
+      <c r="G14" s="164" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="120"/>
+      <c r="H14" s="146"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="86"/>
@@ -2940,14 +2883,14 @@
     <row r="15" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A15" s="29"/>
       <c r="B15" s="30"/>
-      <c r="C15" s="111"/>
+      <c r="C15" s="137"/>
       <c r="D15" s="96" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="137"/>
-      <c r="F15" s="114"/>
-      <c r="G15" s="138"/>
-      <c r="H15" s="127"/>
+      <c r="E15" s="163"/>
+      <c r="F15" s="140"/>
+      <c r="G15" s="164"/>
+      <c r="H15" s="153"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="86"/>
@@ -2962,14 +2905,14 @@
     <row r="16" spans="1:18" s="7" customFormat="1" ht="24.75" customHeight="1">
       <c r="A16" s="29"/>
       <c r="B16" s="30"/>
-      <c r="C16" s="111"/>
+      <c r="C16" s="137"/>
       <c r="D16" s="96" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="123"/>
+      <c r="F16" s="149"/>
       <c r="G16" s="100" t="s">
         <v>14</v>
       </c>
@@ -3010,22 +2953,22 @@
     <row r="18" spans="1:18" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A18" s="29"/>
       <c r="B18" s="30"/>
-      <c r="C18" s="111" t="s">
+      <c r="C18" s="137" t="s">
         <v>199</v>
       </c>
-      <c r="D18" s="116" t="s">
+      <c r="D18" s="142" t="s">
         <v>70</v>
       </c>
       <c r="E18" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="113">
+      <c r="F18" s="139">
         <v>0</v>
       </c>
-      <c r="G18" s="118" t="s">
+      <c r="G18" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="120"/>
+      <c r="H18" s="146"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="86"/>
@@ -3040,14 +2983,14 @@
     <row r="19" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A19" s="29"/>
       <c r="B19" s="30"/>
-      <c r="C19" s="111"/>
-      <c r="D19" s="116"/>
+      <c r="C19" s="137"/>
+      <c r="D19" s="142"/>
       <c r="E19" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="114"/>
-      <c r="G19" s="118"/>
-      <c r="H19" s="121"/>
+      <c r="F19" s="140"/>
+      <c r="G19" s="144"/>
+      <c r="H19" s="147"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="86"/>
@@ -3062,14 +3005,14 @@
     <row r="20" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A20" s="29"/>
       <c r="B20" s="30"/>
-      <c r="C20" s="111"/>
-      <c r="D20" s="116"/>
+      <c r="C20" s="137"/>
+      <c r="D20" s="142"/>
       <c r="E20" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="114"/>
-      <c r="G20" s="118"/>
-      <c r="H20" s="121"/>
+      <c r="F20" s="140"/>
+      <c r="G20" s="144"/>
+      <c r="H20" s="147"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="86"/>
@@ -3084,14 +3027,14 @@
     <row r="21" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A21" s="29"/>
       <c r="B21" s="30"/>
-      <c r="C21" s="111"/>
-      <c r="D21" s="116"/>
+      <c r="C21" s="137"/>
+      <c r="D21" s="142"/>
       <c r="E21" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="114"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="127"/>
+      <c r="F21" s="140"/>
+      <c r="G21" s="144"/>
+      <c r="H21" s="153"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="86"/>
@@ -3106,18 +3049,18 @@
     <row r="22" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A22" s="29"/>
       <c r="B22" s="30"/>
-      <c r="C22" s="111"/>
-      <c r="D22" s="116" t="s">
+      <c r="C22" s="137"/>
+      <c r="D22" s="142" t="s">
         <v>28</v>
       </c>
       <c r="E22" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="114"/>
-      <c r="G22" s="118" t="s">
+      <c r="F22" s="140"/>
+      <c r="G22" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="120"/>
+      <c r="H22" s="146"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="86"/>
@@ -3132,14 +3075,14 @@
     <row r="23" spans="1:18" s="7" customFormat="1" ht="25.5" customHeight="1">
       <c r="A23" s="29"/>
       <c r="B23" s="30"/>
-      <c r="C23" s="111"/>
-      <c r="D23" s="116"/>
+      <c r="C23" s="137"/>
+      <c r="D23" s="142"/>
       <c r="E23" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="114"/>
-      <c r="G23" s="118"/>
-      <c r="H23" s="121"/>
+      <c r="F23" s="140"/>
+      <c r="G23" s="144"/>
+      <c r="H23" s="147"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="86"/>
@@ -3154,14 +3097,14 @@
     <row r="24" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A24" s="29"/>
       <c r="B24" s="30"/>
-      <c r="C24" s="111"/>
-      <c r="D24" s="116"/>
+      <c r="C24" s="137"/>
+      <c r="D24" s="142"/>
       <c r="E24" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="114"/>
-      <c r="G24" s="118"/>
-      <c r="H24" s="121"/>
+      <c r="F24" s="140"/>
+      <c r="G24" s="144"/>
+      <c r="H24" s="147"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
       <c r="K24" s="86"/>
@@ -3176,14 +3119,14 @@
     <row r="25" spans="1:18" s="7" customFormat="1" ht="36" customHeight="1">
       <c r="A25" s="29"/>
       <c r="B25" s="30"/>
-      <c r="C25" s="111"/>
-      <c r="D25" s="116"/>
+      <c r="C25" s="137"/>
+      <c r="D25" s="142"/>
       <c r="E25" s="99" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="114"/>
-      <c r="G25" s="118"/>
-      <c r="H25" s="121"/>
+      <c r="F25" s="140"/>
+      <c r="G25" s="144"/>
+      <c r="H25" s="147"/>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
       <c r="K25" s="86"/>
@@ -3198,14 +3141,14 @@
     <row r="26" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A26" s="29"/>
       <c r="B26" s="30"/>
-      <c r="C26" s="111"/>
-      <c r="D26" s="116"/>
+      <c r="C26" s="137"/>
+      <c r="D26" s="142"/>
       <c r="E26" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="114"/>
-      <c r="G26" s="118"/>
-      <c r="H26" s="127"/>
+      <c r="F26" s="140"/>
+      <c r="G26" s="144"/>
+      <c r="H26" s="153"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="86"/>
@@ -3220,12 +3163,12 @@
     <row r="27" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A27" s="29"/>
       <c r="B27" s="30"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="116"/>
+      <c r="C27" s="137"/>
+      <c r="D27" s="142"/>
       <c r="E27" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="114"/>
+      <c r="F27" s="140"/>
       <c r="G27" s="97" t="s">
         <v>35</v>
       </c>
@@ -3244,14 +3187,14 @@
     <row r="28" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A28" s="29"/>
       <c r="B28" s="30"/>
-      <c r="C28" s="111"/>
+      <c r="C28" s="137"/>
       <c r="D28" s="96" t="s">
         <v>36</v>
       </c>
       <c r="E28" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="F28" s="114"/>
+      <c r="F28" s="140"/>
       <c r="G28" s="97" t="s">
         <v>35</v>
       </c>
@@ -3270,18 +3213,18 @@
     <row r="29" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A29" s="29"/>
       <c r="B29" s="30"/>
-      <c r="C29" s="111"/>
-      <c r="D29" s="116" t="s">
+      <c r="C29" s="137"/>
+      <c r="D29" s="142" t="s">
         <v>38</v>
       </c>
       <c r="E29" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="114"/>
-      <c r="G29" s="118" t="s">
+      <c r="F29" s="140"/>
+      <c r="G29" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="120"/>
+      <c r="H29" s="146"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="86"/>
@@ -3296,14 +3239,14 @@
     <row r="30" spans="1:18" s="7" customFormat="1" ht="36" customHeight="1">
       <c r="A30" s="29"/>
       <c r="B30" s="30"/>
-      <c r="C30" s="111"/>
-      <c r="D30" s="116"/>
+      <c r="C30" s="137"/>
+      <c r="D30" s="142"/>
       <c r="E30" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="F30" s="114"/>
-      <c r="G30" s="118"/>
-      <c r="H30" s="127"/>
+      <c r="F30" s="140"/>
+      <c r="G30" s="144"/>
+      <c r="H30" s="153"/>
       <c r="I30" s="18"/>
       <c r="J30" s="18"/>
       <c r="K30" s="86"/>
@@ -3318,14 +3261,14 @@
     <row r="31" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A31" s="29"/>
       <c r="B31" s="30"/>
-      <c r="C31" s="111"/>
+      <c r="C31" s="137"/>
       <c r="D31" s="96" t="s">
         <v>41</v>
       </c>
       <c r="E31" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="114"/>
+      <c r="F31" s="140"/>
       <c r="G31" s="97" t="s">
         <v>14</v>
       </c>
@@ -3344,18 +3287,18 @@
     <row r="32" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A32" s="29"/>
       <c r="B32" s="30"/>
-      <c r="C32" s="111"/>
-      <c r="D32" s="116" t="s">
+      <c r="C32" s="137"/>
+      <c r="D32" s="142" t="s">
         <v>43</v>
       </c>
       <c r="E32" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F32" s="114"/>
-      <c r="G32" s="118" t="s">
+      <c r="F32" s="140"/>
+      <c r="G32" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="H32" s="120"/>
+      <c r="H32" s="146"/>
       <c r="I32" s="18"/>
       <c r="J32" s="18"/>
       <c r="K32" s="86"/>
@@ -3370,14 +3313,14 @@
     <row r="33" spans="1:18" s="7" customFormat="1" ht="25.5" customHeight="1">
       <c r="A33" s="29"/>
       <c r="B33" s="30"/>
-      <c r="C33" s="111"/>
-      <c r="D33" s="116"/>
+      <c r="C33" s="137"/>
+      <c r="D33" s="142"/>
       <c r="E33" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="F33" s="114"/>
-      <c r="G33" s="118"/>
-      <c r="H33" s="127"/>
+      <c r="F33" s="140"/>
+      <c r="G33" s="144"/>
+      <c r="H33" s="153"/>
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
       <c r="K33" s="86"/>
@@ -3392,12 +3335,12 @@
     <row r="34" spans="1:18" s="7" customFormat="1" ht="26.25" customHeight="1">
       <c r="A34" s="29"/>
       <c r="B34" s="30"/>
-      <c r="C34" s="111"/>
-      <c r="D34" s="116"/>
+      <c r="C34" s="137"/>
+      <c r="D34" s="142"/>
       <c r="E34" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="F34" s="114"/>
+      <c r="F34" s="140"/>
       <c r="G34" s="100"/>
       <c r="H34" s="98" t="s">
         <v>14</v>
@@ -3416,18 +3359,18 @@
     <row r="35" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A35" s="29"/>
       <c r="B35" s="30"/>
-      <c r="C35" s="111"/>
+      <c r="C35" s="137"/>
       <c r="D35" s="96" t="s">
         <v>47</v>
       </c>
-      <c r="E35" s="137" t="s">
+      <c r="E35" s="163" t="s">
         <v>49</v>
       </c>
-      <c r="F35" s="114"/>
-      <c r="G35" s="118" t="s">
+      <c r="F35" s="140"/>
+      <c r="G35" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="H35" s="120"/>
+      <c r="H35" s="146"/>
       <c r="I35" s="18"/>
       <c r="J35" s="18"/>
       <c r="K35" s="86"/>
@@ -3442,14 +3385,14 @@
     <row r="36" spans="1:18" s="7" customFormat="1" ht="36.75" customHeight="1">
       <c r="A36" s="29"/>
       <c r="B36" s="30"/>
-      <c r="C36" s="111"/>
+      <c r="C36" s="137"/>
       <c r="D36" s="96" t="s">
         <v>48</v>
       </c>
-      <c r="E36" s="137"/>
-      <c r="F36" s="114"/>
-      <c r="G36" s="118"/>
-      <c r="H36" s="127"/>
+      <c r="E36" s="163"/>
+      <c r="F36" s="140"/>
+      <c r="G36" s="144"/>
+      <c r="H36" s="153"/>
       <c r="I36" s="18"/>
       <c r="J36" s="18"/>
       <c r="K36" s="86"/>
@@ -3464,14 +3407,14 @@
     <row r="37" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A37" s="29"/>
       <c r="B37" s="30"/>
-      <c r="C37" s="111"/>
+      <c r="C37" s="137"/>
       <c r="D37" s="96" t="s">
         <v>50</v>
       </c>
       <c r="E37" s="99" t="s">
         <v>51</v>
       </c>
-      <c r="F37" s="114"/>
+      <c r="F37" s="140"/>
       <c r="G37" s="100"/>
       <c r="H37" s="98" t="s">
         <v>52</v>
@@ -3490,14 +3433,14 @@
     <row r="38" spans="1:18" s="7" customFormat="1" ht="36" customHeight="1">
       <c r="A38" s="29"/>
       <c r="B38" s="30"/>
-      <c r="C38" s="111"/>
-      <c r="D38" s="116" t="s">
+      <c r="C38" s="137"/>
+      <c r="D38" s="142" t="s">
         <v>53</v>
       </c>
       <c r="E38" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="F38" s="114"/>
+      <c r="F38" s="140"/>
       <c r="G38" s="97" t="s">
         <v>14</v>
       </c>
@@ -3516,12 +3459,12 @@
     <row r="39" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A39" s="29"/>
       <c r="B39" s="30"/>
-      <c r="C39" s="111"/>
-      <c r="D39" s="116"/>
+      <c r="C39" s="137"/>
+      <c r="D39" s="142"/>
       <c r="E39" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="F39" s="114"/>
+      <c r="F39" s="140"/>
       <c r="G39" s="100"/>
       <c r="H39" s="98" t="s">
         <v>52</v>
@@ -3540,14 +3483,14 @@
     <row r="40" spans="1:18" s="7" customFormat="1" ht="25.5" customHeight="1">
       <c r="A40" s="29"/>
       <c r="B40" s="30"/>
-      <c r="C40" s="111"/>
-      <c r="D40" s="116" t="s">
+      <c r="C40" s="137"/>
+      <c r="D40" s="142" t="s">
         <v>56</v>
       </c>
       <c r="E40" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="F40" s="114"/>
+      <c r="F40" s="140"/>
       <c r="G40" s="97" t="s">
         <v>14</v>
       </c>
@@ -3566,12 +3509,12 @@
     <row r="41" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A41" s="29"/>
       <c r="B41" s="30"/>
-      <c r="C41" s="111"/>
-      <c r="D41" s="116"/>
+      <c r="C41" s="137"/>
+      <c r="D41" s="142"/>
       <c r="E41" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="F41" s="114"/>
+      <c r="F41" s="140"/>
       <c r="G41" s="100"/>
       <c r="H41" s="98" t="s">
         <v>52</v>
@@ -3590,14 +3533,14 @@
     <row r="42" spans="1:18" s="7" customFormat="1" ht="36.75" customHeight="1">
       <c r="A42" s="29"/>
       <c r="B42" s="30"/>
-      <c r="C42" s="111"/>
+      <c r="C42" s="137"/>
       <c r="D42" s="96" t="s">
         <v>58</v>
       </c>
       <c r="E42" s="99" t="s">
         <v>59</v>
       </c>
-      <c r="F42" s="114"/>
+      <c r="F42" s="140"/>
       <c r="G42" s="97" t="s">
         <v>52</v>
       </c>
@@ -3616,14 +3559,14 @@
     <row r="43" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A43" s="29"/>
       <c r="B43" s="30"/>
-      <c r="C43" s="111"/>
+      <c r="C43" s="137"/>
       <c r="D43" s="96" t="s">
         <v>60</v>
       </c>
       <c r="E43" s="99" t="s">
         <v>61</v>
       </c>
-      <c r="F43" s="114"/>
+      <c r="F43" s="140"/>
       <c r="G43" s="97" t="s">
         <v>14</v>
       </c>
@@ -3642,14 +3585,14 @@
     <row r="44" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A44" s="29"/>
       <c r="B44" s="30"/>
-      <c r="C44" s="111"/>
+      <c r="C44" s="137"/>
       <c r="D44" s="96" t="s">
         <v>62</v>
       </c>
       <c r="E44" s="99" t="s">
         <v>63</v>
       </c>
-      <c r="F44" s="114"/>
+      <c r="F44" s="140"/>
       <c r="G44" s="100"/>
       <c r="H44" s="98" t="s">
         <v>35</v>
@@ -3668,16 +3611,16 @@
     <row r="45" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A45" s="29"/>
       <c r="B45" s="30"/>
-      <c r="C45" s="111"/>
-      <c r="D45" s="116" t="s">
+      <c r="C45" s="137"/>
+      <c r="D45" s="142" t="s">
         <v>71</v>
       </c>
       <c r="E45" s="99" t="s">
         <v>64</v>
       </c>
-      <c r="F45" s="114"/>
-      <c r="G45" s="124"/>
-      <c r="H45" s="126" t="s">
+      <c r="F45" s="140"/>
+      <c r="G45" s="150"/>
+      <c r="H45" s="152" t="s">
         <v>52</v>
       </c>
       <c r="I45" s="17"/>
@@ -3694,14 +3637,14 @@
     <row r="46" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A46" s="29"/>
       <c r="B46" s="30"/>
-      <c r="C46" s="111"/>
-      <c r="D46" s="116"/>
+      <c r="C46" s="137"/>
+      <c r="D46" s="142"/>
       <c r="E46" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="F46" s="114"/>
-      <c r="G46" s="128"/>
-      <c r="H46" s="126"/>
+      <c r="F46" s="140"/>
+      <c r="G46" s="154"/>
+      <c r="H46" s="152"/>
       <c r="I46" s="17"/>
       <c r="J46" s="17"/>
       <c r="K46" s="85"/>
@@ -3716,14 +3659,14 @@
     <row r="47" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A47" s="29"/>
       <c r="B47" s="30"/>
-      <c r="C47" s="111"/>
-      <c r="D47" s="116"/>
+      <c r="C47" s="137"/>
+      <c r="D47" s="142"/>
       <c r="E47" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="F47" s="114"/>
-      <c r="G47" s="128"/>
-      <c r="H47" s="126"/>
+      <c r="F47" s="140"/>
+      <c r="G47" s="154"/>
+      <c r="H47" s="152"/>
       <c r="I47" s="17"/>
       <c r="J47" s="17"/>
       <c r="K47" s="85"/>
@@ -3738,14 +3681,14 @@
     <row r="48" spans="1:18" s="7" customFormat="1" ht="36" customHeight="1">
       <c r="A48" s="29"/>
       <c r="B48" s="30"/>
-      <c r="C48" s="111"/>
-      <c r="D48" s="116"/>
+      <c r="C48" s="137"/>
+      <c r="D48" s="142"/>
       <c r="E48" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="F48" s="114"/>
-      <c r="G48" s="125"/>
-      <c r="H48" s="126"/>
+      <c r="F48" s="140"/>
+      <c r="G48" s="151"/>
+      <c r="H48" s="152"/>
       <c r="I48" s="17"/>
       <c r="J48" s="17"/>
       <c r="K48" s="85"/>
@@ -3760,14 +3703,14 @@
     <row r="49" spans="1:18" s="7" customFormat="1" ht="74.25" customHeight="1">
       <c r="A49" s="29"/>
       <c r="B49" s="30"/>
-      <c r="C49" s="111"/>
+      <c r="C49" s="137"/>
       <c r="D49" s="96" t="s">
         <v>68</v>
       </c>
       <c r="E49" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="F49" s="114"/>
+      <c r="F49" s="140"/>
       <c r="G49" s="100"/>
       <c r="H49" s="98" t="s">
         <v>52</v>
@@ -3786,18 +3729,18 @@
     <row r="50" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A50" s="29"/>
       <c r="B50" s="30"/>
-      <c r="C50" s="111"/>
-      <c r="D50" s="116" t="s">
+      <c r="C50" s="137"/>
+      <c r="D50" s="142" t="s">
         <v>72</v>
       </c>
       <c r="E50" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="F50" s="114"/>
-      <c r="G50" s="118" t="s">
+      <c r="F50" s="140"/>
+      <c r="G50" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="H50" s="120"/>
+      <c r="H50" s="146"/>
       <c r="I50" s="18"/>
       <c r="J50" s="18"/>
       <c r="K50" s="86"/>
@@ -3812,14 +3755,14 @@
     <row r="51" spans="1:18" s="7" customFormat="1" ht="25.5" customHeight="1">
       <c r="A51" s="29"/>
       <c r="B51" s="30"/>
-      <c r="C51" s="111"/>
-      <c r="D51" s="116"/>
+      <c r="C51" s="137"/>
+      <c r="D51" s="142"/>
       <c r="E51" s="99" t="s">
         <v>74</v>
       </c>
-      <c r="F51" s="114"/>
-      <c r="G51" s="118"/>
-      <c r="H51" s="127"/>
+      <c r="F51" s="140"/>
+      <c r="G51" s="144"/>
+      <c r="H51" s="153"/>
       <c r="I51" s="18"/>
       <c r="J51" s="18"/>
       <c r="K51" s="86"/>
@@ -3834,16 +3777,16 @@
     <row r="52" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A52" s="29"/>
       <c r="B52" s="30"/>
-      <c r="C52" s="111"/>
-      <c r="D52" s="116" t="s">
+      <c r="C52" s="137"/>
+      <c r="D52" s="142" t="s">
         <v>75</v>
       </c>
       <c r="E52" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="F52" s="114"/>
-      <c r="G52" s="124"/>
-      <c r="H52" s="126" t="s">
+      <c r="F52" s="140"/>
+      <c r="G52" s="150"/>
+      <c r="H52" s="152" t="s">
         <v>14</v>
       </c>
       <c r="I52" s="17"/>
@@ -3860,14 +3803,14 @@
     <row r="53" spans="1:18" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A53" s="29"/>
       <c r="B53" s="30"/>
-      <c r="C53" s="111"/>
-      <c r="D53" s="116"/>
+      <c r="C53" s="137"/>
+      <c r="D53" s="142"/>
       <c r="E53" s="99" t="s">
         <v>77</v>
       </c>
-      <c r="F53" s="114"/>
-      <c r="G53" s="128"/>
-      <c r="H53" s="126"/>
+      <c r="F53" s="140"/>
+      <c r="G53" s="154"/>
+      <c r="H53" s="152"/>
       <c r="I53" s="17"/>
       <c r="J53" s="17"/>
       <c r="K53" s="85"/>
@@ -3882,14 +3825,14 @@
     <row r="54" spans="1:18" s="7" customFormat="1" ht="24.75" customHeight="1">
       <c r="A54" s="29"/>
       <c r="B54" s="30"/>
-      <c r="C54" s="111"/>
-      <c r="D54" s="116"/>
+      <c r="C54" s="137"/>
+      <c r="D54" s="142"/>
       <c r="E54" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="F54" s="123"/>
-      <c r="G54" s="125"/>
-      <c r="H54" s="126"/>
+      <c r="F54" s="149"/>
+      <c r="G54" s="151"/>
+      <c r="H54" s="152"/>
       <c r="I54" s="17"/>
       <c r="J54" s="17"/>
       <c r="K54" s="85"/>
@@ -3926,22 +3869,22 @@
     <row r="56" spans="1:18" s="7" customFormat="1" ht="25.5" customHeight="1">
       <c r="A56" s="29"/>
       <c r="B56" s="30"/>
-      <c r="C56" s="111" t="s">
+      <c r="C56" s="137" t="s">
         <v>200</v>
       </c>
-      <c r="D56" s="116" t="s">
+      <c r="D56" s="142" t="s">
         <v>80</v>
       </c>
       <c r="E56" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="F56" s="113">
+      <c r="F56" s="139">
         <v>0</v>
       </c>
-      <c r="G56" s="118" t="s">
+      <c r="G56" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="H56" s="120"/>
+      <c r="H56" s="146"/>
       <c r="I56" s="18"/>
       <c r="J56" s="18"/>
       <c r="K56" s="86"/>
@@ -3956,14 +3899,14 @@
     <row r="57" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A57" s="29"/>
       <c r="B57" s="30"/>
-      <c r="C57" s="111"/>
-      <c r="D57" s="116"/>
+      <c r="C57" s="137"/>
+      <c r="D57" s="142"/>
       <c r="E57" s="99" t="s">
         <v>82</v>
       </c>
-      <c r="F57" s="114"/>
-      <c r="G57" s="118"/>
-      <c r="H57" s="121"/>
+      <c r="F57" s="140"/>
+      <c r="G57" s="144"/>
+      <c r="H57" s="147"/>
       <c r="I57" s="18"/>
       <c r="J57" s="18"/>
       <c r="K57" s="86"/>
@@ -3978,14 +3921,14 @@
     <row r="58" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A58" s="29"/>
       <c r="B58" s="30"/>
-      <c r="C58" s="111"/>
-      <c r="D58" s="116"/>
+      <c r="C58" s="137"/>
+      <c r="D58" s="142"/>
       <c r="E58" s="99" t="s">
         <v>83</v>
       </c>
-      <c r="F58" s="114"/>
-      <c r="G58" s="118"/>
-      <c r="H58" s="121"/>
+      <c r="F58" s="140"/>
+      <c r="G58" s="144"/>
+      <c r="H58" s="147"/>
       <c r="I58" s="18"/>
       <c r="J58" s="18"/>
       <c r="K58" s="86"/>
@@ -4000,14 +3943,14 @@
     <row r="59" spans="1:18" s="7" customFormat="1" ht="36" customHeight="1">
       <c r="A59" s="29"/>
       <c r="B59" s="30"/>
-      <c r="C59" s="111"/>
-      <c r="D59" s="116"/>
+      <c r="C59" s="137"/>
+      <c r="D59" s="142"/>
       <c r="E59" s="99" t="s">
         <v>84</v>
       </c>
-      <c r="F59" s="114"/>
-      <c r="G59" s="118"/>
-      <c r="H59" s="121"/>
+      <c r="F59" s="140"/>
+      <c r="G59" s="144"/>
+      <c r="H59" s="147"/>
       <c r="I59" s="18"/>
       <c r="J59" s="18"/>
       <c r="K59" s="86"/>
@@ -4022,14 +3965,14 @@
     <row r="60" spans="1:18" s="7" customFormat="1" ht="36" customHeight="1">
       <c r="A60" s="29"/>
       <c r="B60" s="30"/>
-      <c r="C60" s="111"/>
-      <c r="D60" s="116"/>
+      <c r="C60" s="137"/>
+      <c r="D60" s="142"/>
       <c r="E60" s="99" t="s">
         <v>85</v>
       </c>
-      <c r="F60" s="114"/>
-      <c r="G60" s="118"/>
-      <c r="H60" s="127"/>
+      <c r="F60" s="140"/>
+      <c r="G60" s="144"/>
+      <c r="H60" s="153"/>
       <c r="I60" s="18"/>
       <c r="J60" s="18"/>
       <c r="K60" s="86"/>
@@ -4044,12 +3987,12 @@
     <row r="61" spans="1:18" s="7" customFormat="1" ht="24.75" customHeight="1">
       <c r="A61" s="29"/>
       <c r="B61" s="30"/>
-      <c r="C61" s="111"/>
-      <c r="D61" s="116"/>
+      <c r="C61" s="137"/>
+      <c r="D61" s="142"/>
       <c r="E61" s="99" t="s">
         <v>86</v>
       </c>
-      <c r="F61" s="123"/>
+      <c r="F61" s="149"/>
       <c r="G61" s="100"/>
       <c r="H61" s="98" t="s">
         <v>14</v>
@@ -4132,22 +4075,22 @@
     <row r="65" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A65" s="29"/>
       <c r="B65" s="30"/>
-      <c r="C65" s="111" t="s">
+      <c r="C65" s="137" t="s">
         <v>201</v>
       </c>
-      <c r="D65" s="116" t="s">
+      <c r="D65" s="142" t="s">
         <v>88</v>
       </c>
       <c r="E65" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="F65" s="113">
+      <c r="F65" s="139">
         <v>0</v>
       </c>
-      <c r="G65" s="118" t="s">
+      <c r="G65" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="H65" s="120"/>
+      <c r="H65" s="146"/>
       <c r="I65" s="18"/>
       <c r="J65" s="18"/>
       <c r="K65" s="86"/>
@@ -4162,14 +4105,14 @@
     <row r="66" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A66" s="29"/>
       <c r="B66" s="30"/>
-      <c r="C66" s="111"/>
-      <c r="D66" s="116"/>
+      <c r="C66" s="137"/>
+      <c r="D66" s="142"/>
       <c r="E66" s="99" t="s">
         <v>90</v>
       </c>
-      <c r="F66" s="114"/>
-      <c r="G66" s="118"/>
-      <c r="H66" s="127"/>
+      <c r="F66" s="140"/>
+      <c r="G66" s="144"/>
+      <c r="H66" s="153"/>
       <c r="I66" s="18"/>
       <c r="J66" s="18"/>
       <c r="K66" s="86"/>
@@ -4184,16 +4127,16 @@
     <row r="67" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A67" s="29"/>
       <c r="B67" s="30"/>
-      <c r="C67" s="111"/>
-      <c r="D67" s="116" t="s">
+      <c r="C67" s="137"/>
+      <c r="D67" s="142" t="s">
         <v>91</v>
       </c>
       <c r="E67" s="99" t="s">
         <v>92</v>
       </c>
-      <c r="F67" s="114"/>
-      <c r="G67" s="124"/>
-      <c r="H67" s="126" t="s">
+      <c r="F67" s="140"/>
+      <c r="G67" s="150"/>
+      <c r="H67" s="152" t="s">
         <v>14</v>
       </c>
       <c r="I67" s="17"/>
@@ -4210,14 +4153,14 @@
     <row r="68" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A68" s="29"/>
       <c r="B68" s="30"/>
-      <c r="C68" s="111"/>
-      <c r="D68" s="116"/>
+      <c r="C68" s="137"/>
+      <c r="D68" s="142"/>
       <c r="E68" s="99" t="s">
         <v>93</v>
       </c>
-      <c r="F68" s="114"/>
-      <c r="G68" s="128"/>
-      <c r="H68" s="126"/>
+      <c r="F68" s="140"/>
+      <c r="G68" s="154"/>
+      <c r="H68" s="152"/>
       <c r="I68" s="17"/>
       <c r="J68" s="17"/>
       <c r="K68" s="85"/>
@@ -4232,14 +4175,14 @@
     <row r="69" spans="1:18" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A69" s="29"/>
       <c r="B69" s="30"/>
-      <c r="C69" s="111"/>
-      <c r="D69" s="116"/>
+      <c r="C69" s="137"/>
+      <c r="D69" s="142"/>
       <c r="E69" s="99" t="s">
         <v>94</v>
       </c>
-      <c r="F69" s="114"/>
-      <c r="G69" s="128"/>
-      <c r="H69" s="126"/>
+      <c r="F69" s="140"/>
+      <c r="G69" s="154"/>
+      <c r="H69" s="152"/>
       <c r="I69" s="17"/>
       <c r="J69" s="17"/>
       <c r="K69" s="85"/>
@@ -4254,14 +4197,14 @@
     <row r="70" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A70" s="29"/>
       <c r="B70" s="30"/>
-      <c r="C70" s="111"/>
-      <c r="D70" s="116"/>
+      <c r="C70" s="137"/>
+      <c r="D70" s="142"/>
       <c r="E70" s="99" t="s">
         <v>95</v>
       </c>
-      <c r="F70" s="114"/>
-      <c r="G70" s="125"/>
-      <c r="H70" s="126"/>
+      <c r="F70" s="140"/>
+      <c r="G70" s="151"/>
+      <c r="H70" s="152"/>
       <c r="I70" s="17"/>
       <c r="J70" s="17"/>
       <c r="K70" s="85"/>
@@ -4276,14 +4219,14 @@
     <row r="71" spans="1:18" s="7" customFormat="1" ht="25.5" customHeight="1">
       <c r="A71" s="29"/>
       <c r="B71" s="30"/>
-      <c r="C71" s="111"/>
+      <c r="C71" s="137"/>
       <c r="D71" s="96" t="s">
         <v>72</v>
       </c>
       <c r="E71" s="99" t="s">
         <v>96</v>
       </c>
-      <c r="F71" s="114"/>
+      <c r="F71" s="140"/>
       <c r="G71" s="100"/>
       <c r="H71" s="98" t="s">
         <v>14</v>
@@ -4302,16 +4245,16 @@
     <row r="72" spans="1:18" s="7" customFormat="1" ht="36" customHeight="1">
       <c r="A72" s="29"/>
       <c r="B72" s="30"/>
-      <c r="C72" s="111"/>
-      <c r="D72" s="116" t="s">
+      <c r="C72" s="137"/>
+      <c r="D72" s="142" t="s">
         <v>103</v>
       </c>
       <c r="E72" s="99" t="s">
         <v>97</v>
       </c>
-      <c r="F72" s="114"/>
-      <c r="G72" s="124"/>
-      <c r="H72" s="126" t="s">
+      <c r="F72" s="140"/>
+      <c r="G72" s="150"/>
+      <c r="H72" s="152" t="s">
         <v>14</v>
       </c>
       <c r="I72" s="17"/>
@@ -4328,14 +4271,14 @@
     <row r="73" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A73" s="29"/>
       <c r="B73" s="30"/>
-      <c r="C73" s="111"/>
-      <c r="D73" s="116"/>
+      <c r="C73" s="137"/>
+      <c r="D73" s="142"/>
       <c r="E73" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="F73" s="114"/>
-      <c r="G73" s="125"/>
-      <c r="H73" s="126"/>
+      <c r="F73" s="140"/>
+      <c r="G73" s="151"/>
+      <c r="H73" s="152"/>
       <c r="I73" s="17"/>
       <c r="J73" s="17"/>
       <c r="K73" s="85"/>
@@ -4350,14 +4293,14 @@
     <row r="74" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A74" s="29"/>
       <c r="B74" s="30"/>
-      <c r="C74" s="111"/>
+      <c r="C74" s="137"/>
       <c r="D74" s="96" t="s">
         <v>99</v>
       </c>
       <c r="E74" s="99" t="s">
         <v>100</v>
       </c>
-      <c r="F74" s="114"/>
+      <c r="F74" s="140"/>
       <c r="G74" s="100"/>
       <c r="H74" s="98" t="s">
         <v>14</v>
@@ -4376,14 +4319,14 @@
     <row r="75" spans="1:18" s="7" customFormat="1" ht="24.75" customHeight="1">
       <c r="A75" s="29"/>
       <c r="B75" s="30"/>
-      <c r="C75" s="111"/>
+      <c r="C75" s="137"/>
       <c r="D75" s="96" t="s">
         <v>101</v>
       </c>
       <c r="E75" s="99" t="s">
         <v>102</v>
       </c>
-      <c r="F75" s="123"/>
+      <c r="F75" s="149"/>
       <c r="G75" s="97" t="s">
         <v>14</v>
       </c>
@@ -4424,16 +4367,16 @@
     <row r="77" spans="1:18" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A77" s="29"/>
       <c r="B77" s="30"/>
-      <c r="C77" s="111" t="s">
+      <c r="C77" s="137" t="s">
         <v>202</v>
       </c>
-      <c r="D77" s="116" t="s">
+      <c r="D77" s="142" t="s">
         <v>43</v>
       </c>
       <c r="E77" s="99" t="s">
         <v>105</v>
       </c>
-      <c r="F77" s="113">
+      <c r="F77" s="139">
         <v>0</v>
       </c>
       <c r="G77" s="97" t="s">
@@ -4454,14 +4397,14 @@
     <row r="78" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A78" s="29"/>
       <c r="B78" s="30"/>
-      <c r="C78" s="111"/>
-      <c r="D78" s="116"/>
+      <c r="C78" s="137"/>
+      <c r="D78" s="142"/>
       <c r="E78" s="99" t="s">
         <v>106</v>
       </c>
-      <c r="F78" s="114"/>
-      <c r="G78" s="124"/>
-      <c r="H78" s="126" t="s">
+      <c r="F78" s="140"/>
+      <c r="G78" s="150"/>
+      <c r="H78" s="152" t="s">
         <v>14</v>
       </c>
       <c r="I78" s="17"/>
@@ -4478,14 +4421,14 @@
     <row r="79" spans="1:18" s="7" customFormat="1" ht="36" customHeight="1">
       <c r="A79" s="29"/>
       <c r="B79" s="30"/>
-      <c r="C79" s="111"/>
-      <c r="D79" s="116"/>
+      <c r="C79" s="137"/>
+      <c r="D79" s="142"/>
       <c r="E79" s="99" t="s">
         <v>107</v>
       </c>
-      <c r="F79" s="114"/>
-      <c r="G79" s="125"/>
-      <c r="H79" s="126"/>
+      <c r="F79" s="140"/>
+      <c r="G79" s="151"/>
+      <c r="H79" s="152"/>
       <c r="I79" s="17"/>
       <c r="J79" s="17"/>
       <c r="K79" s="85"/>
@@ -4500,14 +4443,14 @@
     <row r="80" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A80" s="29"/>
       <c r="B80" s="30"/>
-      <c r="C80" s="111"/>
+      <c r="C80" s="137"/>
       <c r="D80" s="96" t="s">
         <v>41</v>
       </c>
       <c r="E80" s="99" t="s">
         <v>108</v>
       </c>
-      <c r="F80" s="114"/>
+      <c r="F80" s="140"/>
       <c r="G80" s="100"/>
       <c r="H80" s="98" t="s">
         <v>14</v>
@@ -4526,16 +4469,16 @@
     <row r="81" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A81" s="29"/>
       <c r="B81" s="30"/>
-      <c r="C81" s="111"/>
-      <c r="D81" s="129" t="s">
+      <c r="C81" s="137"/>
+      <c r="D81" s="155" t="s">
         <v>109</v>
       </c>
       <c r="E81" s="99" t="s">
         <v>110</v>
       </c>
-      <c r="F81" s="114"/>
-      <c r="G81" s="124"/>
-      <c r="H81" s="126" t="s">
+      <c r="F81" s="140"/>
+      <c r="G81" s="150"/>
+      <c r="H81" s="152" t="s">
         <v>52</v>
       </c>
       <c r="I81" s="17"/>
@@ -4552,14 +4495,14 @@
     <row r="82" spans="1:18" s="7" customFormat="1" ht="25.5" customHeight="1">
       <c r="A82" s="29"/>
       <c r="B82" s="30"/>
-      <c r="C82" s="111"/>
-      <c r="D82" s="130"/>
+      <c r="C82" s="137"/>
+      <c r="D82" s="156"/>
       <c r="E82" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="F82" s="114"/>
-      <c r="G82" s="125"/>
-      <c r="H82" s="126"/>
+      <c r="F82" s="140"/>
+      <c r="G82" s="151"/>
+      <c r="H82" s="152"/>
       <c r="I82" s="17"/>
       <c r="J82" s="17"/>
       <c r="K82" s="85"/>
@@ -4574,14 +4517,14 @@
     <row r="83" spans="1:18" s="7" customFormat="1" ht="60.75" customHeight="1">
       <c r="A83" s="29"/>
       <c r="B83" s="30"/>
-      <c r="C83" s="111"/>
+      <c r="C83" s="137"/>
       <c r="D83" s="96" t="s">
         <v>131</v>
       </c>
       <c r="E83" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="F83" s="114"/>
+      <c r="F83" s="140"/>
       <c r="G83" s="100"/>
       <c r="H83" s="98" t="s">
         <v>14</v>
@@ -4600,18 +4543,18 @@
     <row r="84" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A84" s="29"/>
       <c r="B84" s="30"/>
-      <c r="C84" s="111"/>
-      <c r="D84" s="116" t="s">
+      <c r="C84" s="137"/>
+      <c r="D84" s="142" t="s">
         <v>113</v>
       </c>
       <c r="E84" s="99" t="s">
         <v>114</v>
       </c>
-      <c r="F84" s="114"/>
-      <c r="G84" s="118" t="s">
+      <c r="F84" s="140"/>
+      <c r="G84" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="H84" s="120"/>
+      <c r="H84" s="146"/>
       <c r="I84" s="18"/>
       <c r="J84" s="18"/>
       <c r="K84" s="86"/>
@@ -4626,14 +4569,14 @@
     <row r="85" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A85" s="29"/>
       <c r="B85" s="30"/>
-      <c r="C85" s="111"/>
-      <c r="D85" s="116"/>
+      <c r="C85" s="137"/>
+      <c r="D85" s="142"/>
       <c r="E85" s="99" t="s">
         <v>115</v>
       </c>
-      <c r="F85" s="114"/>
-      <c r="G85" s="118"/>
-      <c r="H85" s="121"/>
+      <c r="F85" s="140"/>
+      <c r="G85" s="144"/>
+      <c r="H85" s="147"/>
       <c r="I85" s="18"/>
       <c r="J85" s="18"/>
       <c r="K85" s="86"/>
@@ -4648,14 +4591,14 @@
     <row r="86" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A86" s="29"/>
       <c r="B86" s="30"/>
-      <c r="C86" s="111"/>
-      <c r="D86" s="116"/>
+      <c r="C86" s="137"/>
+      <c r="D86" s="142"/>
       <c r="E86" s="99" t="s">
         <v>116</v>
       </c>
-      <c r="F86" s="114"/>
-      <c r="G86" s="118"/>
-      <c r="H86" s="127"/>
+      <c r="F86" s="140"/>
+      <c r="G86" s="144"/>
+      <c r="H86" s="153"/>
       <c r="I86" s="18"/>
       <c r="J86" s="18"/>
       <c r="K86" s="86"/>
@@ -4670,14 +4613,14 @@
     <row r="87" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A87" s="29"/>
       <c r="B87" s="30"/>
-      <c r="C87" s="111"/>
+      <c r="C87" s="137"/>
       <c r="D87" s="96" t="s">
         <v>117</v>
       </c>
       <c r="E87" s="99" t="s">
         <v>118</v>
       </c>
-      <c r="F87" s="114"/>
+      <c r="F87" s="140"/>
       <c r="G87" s="97" t="s">
         <v>14</v>
       </c>
@@ -4696,16 +4639,16 @@
     <row r="88" spans="1:18" s="7" customFormat="1" ht="25.5" customHeight="1">
       <c r="A88" s="29"/>
       <c r="B88" s="30"/>
-      <c r="C88" s="111"/>
-      <c r="D88" s="116" t="s">
+      <c r="C88" s="137"/>
+      <c r="D88" s="142" t="s">
         <v>119</v>
       </c>
       <c r="E88" s="99" t="s">
         <v>120</v>
       </c>
-      <c r="F88" s="114"/>
-      <c r="G88" s="124"/>
-      <c r="H88" s="126" t="s">
+      <c r="F88" s="140"/>
+      <c r="G88" s="150"/>
+      <c r="H88" s="152" t="s">
         <v>14</v>
       </c>
       <c r="I88" s="17"/>
@@ -4722,14 +4665,14 @@
     <row r="89" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A89" s="29"/>
       <c r="B89" s="30"/>
-      <c r="C89" s="111"/>
-      <c r="D89" s="116"/>
+      <c r="C89" s="137"/>
+      <c r="D89" s="142"/>
       <c r="E89" s="99" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="114"/>
-      <c r="G89" s="125"/>
-      <c r="H89" s="126"/>
+      <c r="F89" s="140"/>
+      <c r="G89" s="151"/>
+      <c r="H89" s="152"/>
       <c r="I89" s="17"/>
       <c r="J89" s="17"/>
       <c r="K89" s="85"/>
@@ -4744,14 +4687,14 @@
     <row r="90" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A90" s="29"/>
       <c r="B90" s="30"/>
-      <c r="C90" s="111"/>
+      <c r="C90" s="137"/>
       <c r="D90" s="96" t="s">
         <v>122</v>
       </c>
       <c r="E90" s="99" t="s">
         <v>123</v>
       </c>
-      <c r="F90" s="114"/>
+      <c r="F90" s="140"/>
       <c r="G90" s="100"/>
       <c r="H90" s="98" t="s">
         <v>14</v>
@@ -4770,14 +4713,14 @@
     <row r="91" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A91" s="29"/>
       <c r="B91" s="30"/>
-      <c r="C91" s="111"/>
+      <c r="C91" s="137"/>
       <c r="D91" s="96" t="s">
         <v>124</v>
       </c>
       <c r="E91" s="99" t="s">
         <v>125</v>
       </c>
-      <c r="F91" s="114"/>
+      <c r="F91" s="140"/>
       <c r="G91" s="97" t="s">
         <v>14</v>
       </c>
@@ -4796,16 +4739,16 @@
     <row r="92" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A92" s="29"/>
       <c r="B92" s="30"/>
-      <c r="C92" s="111"/>
-      <c r="D92" s="116" t="s">
+      <c r="C92" s="137"/>
+      <c r="D92" s="142" t="s">
         <v>75</v>
       </c>
       <c r="E92" s="99" t="s">
         <v>126</v>
       </c>
-      <c r="F92" s="114"/>
-      <c r="G92" s="124"/>
-      <c r="H92" s="126" t="s">
+      <c r="F92" s="140"/>
+      <c r="G92" s="150"/>
+      <c r="H92" s="152" t="s">
         <v>52</v>
       </c>
       <c r="I92" s="17"/>
@@ -4822,14 +4765,14 @@
     <row r="93" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A93" s="29"/>
       <c r="B93" s="30"/>
-      <c r="C93" s="111"/>
-      <c r="D93" s="116"/>
+      <c r="C93" s="137"/>
+      <c r="D93" s="142"/>
       <c r="E93" s="99" t="s">
         <v>127</v>
       </c>
-      <c r="F93" s="114"/>
-      <c r="G93" s="128"/>
-      <c r="H93" s="126"/>
+      <c r="F93" s="140"/>
+      <c r="G93" s="154"/>
+      <c r="H93" s="152"/>
       <c r="I93" s="17"/>
       <c r="J93" s="17"/>
       <c r="K93" s="85"/>
@@ -4844,14 +4787,14 @@
     <row r="94" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A94" s="29"/>
       <c r="B94" s="30"/>
-      <c r="C94" s="111"/>
-      <c r="D94" s="116"/>
+      <c r="C94" s="137"/>
+      <c r="D94" s="142"/>
       <c r="E94" s="99" t="s">
         <v>128</v>
       </c>
-      <c r="F94" s="114"/>
-      <c r="G94" s="125"/>
-      <c r="H94" s="126"/>
+      <c r="F94" s="140"/>
+      <c r="G94" s="151"/>
+      <c r="H94" s="152"/>
       <c r="I94" s="17"/>
       <c r="J94" s="17"/>
       <c r="K94" s="85"/>
@@ -4866,14 +4809,14 @@
     <row r="95" spans="1:18" s="7" customFormat="1" ht="24.75" customHeight="1">
       <c r="A95" s="29"/>
       <c r="B95" s="30"/>
-      <c r="C95" s="111"/>
+      <c r="C95" s="137"/>
       <c r="D95" s="96" t="s">
         <v>129</v>
       </c>
       <c r="E95" s="99" t="s">
         <v>130</v>
       </c>
-      <c r="F95" s="123"/>
+      <c r="F95" s="149"/>
       <c r="G95" s="97" t="s">
         <v>14</v>
       </c>
@@ -4914,20 +4857,20 @@
     <row r="97" spans="1:18" s="7" customFormat="1" ht="48.75" customHeight="1">
       <c r="A97" s="29"/>
       <c r="B97" s="30"/>
-      <c r="C97" s="111" t="s">
+      <c r="C97" s="137" t="s">
         <v>203</v>
       </c>
-      <c r="D97" s="116" t="s">
+      <c r="D97" s="142" t="s">
         <v>141</v>
       </c>
       <c r="E97" s="99" t="s">
         <v>133</v>
       </c>
-      <c r="F97" s="113">
+      <c r="F97" s="139">
         <v>0</v>
       </c>
-      <c r="G97" s="124"/>
-      <c r="H97" s="126" t="s">
+      <c r="G97" s="150"/>
+      <c r="H97" s="152" t="s">
         <v>14</v>
       </c>
       <c r="I97" s="17"/>
@@ -4944,14 +4887,14 @@
     <row r="98" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A98" s="29"/>
       <c r="B98" s="30"/>
-      <c r="C98" s="111"/>
-      <c r="D98" s="116"/>
+      <c r="C98" s="137"/>
+      <c r="D98" s="142"/>
       <c r="E98" s="99" t="s">
         <v>134</v>
       </c>
-      <c r="F98" s="114"/>
-      <c r="G98" s="125"/>
-      <c r="H98" s="126"/>
+      <c r="F98" s="140"/>
+      <c r="G98" s="151"/>
+      <c r="H98" s="152"/>
       <c r="I98" s="17"/>
       <c r="J98" s="17"/>
       <c r="K98" s="85"/>
@@ -4966,14 +4909,14 @@
     <row r="99" spans="1:18" s="7" customFormat="1" ht="49.5" customHeight="1">
       <c r="A99" s="29"/>
       <c r="B99" s="30"/>
-      <c r="C99" s="111"/>
+      <c r="C99" s="137"/>
       <c r="D99" s="96" t="s">
         <v>135</v>
       </c>
       <c r="E99" s="99" t="s">
         <v>136</v>
       </c>
-      <c r="F99" s="114"/>
+      <c r="F99" s="140"/>
       <c r="G99" s="100"/>
       <c r="H99" s="98" t="s">
         <v>14</v>
@@ -4992,14 +4935,14 @@
     <row r="100" spans="1:18" s="7" customFormat="1" ht="36" customHeight="1">
       <c r="A100" s="29"/>
       <c r="B100" s="30"/>
-      <c r="C100" s="111"/>
+      <c r="C100" s="137"/>
       <c r="D100" s="96" t="s">
         <v>109</v>
       </c>
       <c r="E100" s="99" t="s">
         <v>137</v>
       </c>
-      <c r="F100" s="114"/>
+      <c r="F100" s="140"/>
       <c r="G100" s="100"/>
       <c r="H100" s="98" t="s">
         <v>52</v>
@@ -5018,16 +4961,16 @@
     <row r="101" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A101" s="29"/>
       <c r="B101" s="30"/>
-      <c r="C101" s="111"/>
-      <c r="D101" s="116" t="s">
+      <c r="C101" s="137"/>
+      <c r="D101" s="142" t="s">
         <v>75</v>
       </c>
       <c r="E101" s="99" t="s">
         <v>138</v>
       </c>
-      <c r="F101" s="114"/>
-      <c r="G101" s="124"/>
-      <c r="H101" s="126" t="s">
+      <c r="F101" s="140"/>
+      <c r="G101" s="150"/>
+      <c r="H101" s="152" t="s">
         <v>14</v>
       </c>
       <c r="I101" s="17"/>
@@ -5044,14 +4987,14 @@
     <row r="102" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A102" s="29"/>
       <c r="B102" s="30"/>
-      <c r="C102" s="111"/>
-      <c r="D102" s="116"/>
+      <c r="C102" s="137"/>
+      <c r="D102" s="142"/>
       <c r="E102" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="F102" s="114"/>
-      <c r="G102" s="128"/>
-      <c r="H102" s="126"/>
+      <c r="F102" s="140"/>
+      <c r="G102" s="154"/>
+      <c r="H102" s="152"/>
       <c r="I102" s="17"/>
       <c r="J102" s="17"/>
       <c r="K102" s="85"/>
@@ -5066,14 +5009,14 @@
     <row r="103" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A103" s="29"/>
       <c r="B103" s="30"/>
-      <c r="C103" s="111"/>
-      <c r="D103" s="116"/>
+      <c r="C103" s="137"/>
+      <c r="D103" s="142"/>
       <c r="E103" s="99" t="s">
         <v>140</v>
       </c>
-      <c r="F103" s="114"/>
-      <c r="G103" s="125"/>
-      <c r="H103" s="126"/>
+      <c r="F103" s="140"/>
+      <c r="G103" s="151"/>
+      <c r="H103" s="152"/>
       <c r="I103" s="17"/>
       <c r="J103" s="17"/>
       <c r="K103" s="85"/>
@@ -5088,14 +5031,14 @@
     <row r="104" spans="1:18" s="7" customFormat="1" ht="24.75" customHeight="1">
       <c r="A104" s="29"/>
       <c r="B104" s="30"/>
-      <c r="C104" s="111"/>
+      <c r="C104" s="137"/>
       <c r="D104" s="96" t="s">
         <v>129</v>
       </c>
       <c r="E104" s="99" t="s">
         <v>142</v>
       </c>
-      <c r="F104" s="123"/>
+      <c r="F104" s="149"/>
       <c r="G104" s="97" t="s">
         <v>14</v>
       </c>
@@ -5136,10 +5079,10 @@
     <row r="106" spans="1:18" s="7" customFormat="1" ht="48" customHeight="1">
       <c r="A106" s="29"/>
       <c r="B106" s="30"/>
-      <c r="C106" s="111" t="s">
+      <c r="C106" s="137" t="s">
         <v>208</v>
       </c>
-      <c r="D106" s="116" t="s">
+      <c r="D106" s="142" t="s">
         <v>144</v>
       </c>
       <c r="E106" s="99" t="s">
@@ -5166,8 +5109,8 @@
     <row r="107" spans="1:18" s="7" customFormat="1" ht="36.75" customHeight="1">
       <c r="A107" s="29"/>
       <c r="B107" s="30"/>
-      <c r="C107" s="111"/>
-      <c r="D107" s="116"/>
+      <c r="C107" s="137"/>
+      <c r="D107" s="142"/>
       <c r="E107" s="99" t="s">
         <v>146</v>
       </c>
@@ -5192,8 +5135,8 @@
     <row r="108" spans="1:18" s="7" customFormat="1" ht="25.5" customHeight="1">
       <c r="A108" s="29"/>
       <c r="B108" s="30"/>
-      <c r="C108" s="111"/>
-      <c r="D108" s="116" t="s">
+      <c r="C108" s="137"/>
+      <c r="D108" s="142" t="s">
         <v>72</v>
       </c>
       <c r="E108" s="99" t="s">
@@ -5202,8 +5145,8 @@
       <c r="F108" s="14">
         <v>0</v>
       </c>
-      <c r="G108" s="124"/>
-      <c r="H108" s="126" t="s">
+      <c r="G108" s="150"/>
+      <c r="H108" s="152" t="s">
         <v>52</v>
       </c>
       <c r="I108" s="17"/>
@@ -5220,16 +5163,16 @@
     <row r="109" spans="1:18" s="7" customFormat="1" ht="25.5" customHeight="1">
       <c r="A109" s="29"/>
       <c r="B109" s="30"/>
-      <c r="C109" s="111"/>
-      <c r="D109" s="116"/>
+      <c r="C109" s="137"/>
+      <c r="D109" s="142"/>
       <c r="E109" s="99" t="s">
         <v>148</v>
       </c>
       <c r="F109" s="14">
         <v>0</v>
       </c>
-      <c r="G109" s="125"/>
-      <c r="H109" s="126"/>
+      <c r="G109" s="151"/>
+      <c r="H109" s="152"/>
       <c r="I109" s="17"/>
       <c r="J109" s="17"/>
       <c r="K109" s="85"/>
@@ -5244,8 +5187,8 @@
     <row r="110" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A110" s="29"/>
       <c r="B110" s="30"/>
-      <c r="C110" s="111"/>
-      <c r="D110" s="116" t="s">
+      <c r="C110" s="137"/>
+      <c r="D110" s="142" t="s">
         <v>149</v>
       </c>
       <c r="E110" s="99" t="s">
@@ -5254,8 +5197,8 @@
       <c r="F110" s="14">
         <v>0</v>
       </c>
-      <c r="G110" s="124"/>
-      <c r="H110" s="126" t="s">
+      <c r="G110" s="150"/>
+      <c r="H110" s="152" t="s">
         <v>14</v>
       </c>
       <c r="I110" s="17"/>
@@ -5272,16 +5215,16 @@
     <row r="111" spans="1:18" s="7" customFormat="1" ht="25.5" customHeight="1">
       <c r="A111" s="29"/>
       <c r="B111" s="30"/>
-      <c r="C111" s="111"/>
-      <c r="D111" s="116"/>
+      <c r="C111" s="137"/>
+      <c r="D111" s="142"/>
       <c r="E111" s="99" t="s">
         <v>151</v>
       </c>
       <c r="F111" s="14">
         <v>0</v>
       </c>
-      <c r="G111" s="125"/>
-      <c r="H111" s="126"/>
+      <c r="G111" s="151"/>
+      <c r="H111" s="152"/>
       <c r="I111" s="17"/>
       <c r="J111" s="17"/>
       <c r="K111" s="85"/>
@@ -5296,7 +5239,7 @@
     <row r="112" spans="1:18" s="7" customFormat="1" ht="24.75" customHeight="1">
       <c r="A112" s="29"/>
       <c r="B112" s="30"/>
-      <c r="C112" s="111"/>
+      <c r="C112" s="137"/>
       <c r="D112" s="96" t="s">
         <v>152</v>
       </c>
@@ -5388,20 +5331,20 @@
     <row r="116" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A116" s="29"/>
       <c r="B116" s="30"/>
-      <c r="C116" s="111" t="s">
+      <c r="C116" s="137" t="s">
         <v>204</v>
       </c>
-      <c r="D116" s="116" t="s">
+      <c r="D116" s="142" t="s">
         <v>155</v>
       </c>
       <c r="E116" s="99" t="s">
         <v>156</v>
       </c>
-      <c r="F116" s="113">
+      <c r="F116" s="139">
         <v>0</v>
       </c>
-      <c r="G116" s="124"/>
-      <c r="H116" s="126" t="s">
+      <c r="G116" s="150"/>
+      <c r="H116" s="152" t="s">
         <v>14</v>
       </c>
       <c r="I116" s="17"/>
@@ -5418,14 +5361,14 @@
     <row r="117" spans="1:18" s="7" customFormat="1" ht="36" customHeight="1">
       <c r="A117" s="29"/>
       <c r="B117" s="30"/>
-      <c r="C117" s="111"/>
-      <c r="D117" s="116"/>
+      <c r="C117" s="137"/>
+      <c r="D117" s="142"/>
       <c r="E117" s="99" t="s">
         <v>157</v>
       </c>
-      <c r="F117" s="114"/>
-      <c r="G117" s="128"/>
-      <c r="H117" s="126"/>
+      <c r="F117" s="140"/>
+      <c r="G117" s="154"/>
+      <c r="H117" s="152"/>
       <c r="I117" s="17"/>
       <c r="J117" s="17"/>
       <c r="K117" s="85"/>
@@ -5440,14 +5383,14 @@
     <row r="118" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A118" s="29"/>
       <c r="B118" s="30"/>
-      <c r="C118" s="111"/>
-      <c r="D118" s="116"/>
+      <c r="C118" s="137"/>
+      <c r="D118" s="142"/>
       <c r="E118" s="99" t="s">
         <v>158</v>
       </c>
-      <c r="F118" s="114"/>
-      <c r="G118" s="125"/>
-      <c r="H118" s="126"/>
+      <c r="F118" s="140"/>
+      <c r="G118" s="151"/>
+      <c r="H118" s="152"/>
       <c r="I118" s="17"/>
       <c r="J118" s="17"/>
       <c r="K118" s="85"/>
@@ -5462,16 +5405,16 @@
     <row r="119" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A119" s="29"/>
       <c r="B119" s="30"/>
-      <c r="C119" s="111"/>
-      <c r="D119" s="116" t="s">
+      <c r="C119" s="137"/>
+      <c r="D119" s="142" t="s">
         <v>159</v>
       </c>
       <c r="E119" s="99" t="s">
         <v>160</v>
       </c>
-      <c r="F119" s="114"/>
-      <c r="G119" s="124"/>
-      <c r="H119" s="126" t="s">
+      <c r="F119" s="140"/>
+      <c r="G119" s="150"/>
+      <c r="H119" s="152" t="s">
         <v>14</v>
       </c>
       <c r="I119" s="17"/>
@@ -5488,14 +5431,14 @@
     <row r="120" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A120" s="29"/>
       <c r="B120" s="30"/>
-      <c r="C120" s="111"/>
-      <c r="D120" s="116"/>
+      <c r="C120" s="137"/>
+      <c r="D120" s="142"/>
       <c r="E120" s="99" t="s">
         <v>161</v>
       </c>
-      <c r="F120" s="114"/>
-      <c r="G120" s="125"/>
-      <c r="H120" s="126"/>
+      <c r="F120" s="140"/>
+      <c r="G120" s="151"/>
+      <c r="H120" s="152"/>
       <c r="I120" s="17"/>
       <c r="J120" s="17"/>
       <c r="K120" s="85"/>
@@ -5510,16 +5453,16 @@
     <row r="121" spans="1:18" s="7" customFormat="1" ht="36" customHeight="1">
       <c r="A121" s="29"/>
       <c r="B121" s="30"/>
-      <c r="C121" s="111"/>
-      <c r="D121" s="116" t="s">
+      <c r="C121" s="137"/>
+      <c r="D121" s="142" t="s">
         <v>162</v>
       </c>
       <c r="E121" s="99" t="s">
         <v>163</v>
       </c>
-      <c r="F121" s="114"/>
-      <c r="G121" s="124"/>
-      <c r="H121" s="126" t="s">
+      <c r="F121" s="140"/>
+      <c r="G121" s="150"/>
+      <c r="H121" s="152" t="s">
         <v>14</v>
       </c>
       <c r="I121" s="17"/>
@@ -5536,14 +5479,14 @@
     <row r="122" spans="1:18" s="7" customFormat="1" ht="24.75" customHeight="1">
       <c r="A122" s="29"/>
       <c r="B122" s="30"/>
-      <c r="C122" s="111"/>
-      <c r="D122" s="116"/>
+      <c r="C122" s="137"/>
+      <c r="D122" s="142"/>
       <c r="E122" s="99" t="s">
         <v>164</v>
       </c>
-      <c r="F122" s="123"/>
-      <c r="G122" s="125"/>
-      <c r="H122" s="126"/>
+      <c r="F122" s="149"/>
+      <c r="G122" s="151"/>
+      <c r="H122" s="152"/>
       <c r="I122" s="17"/>
       <c r="J122" s="17"/>
       <c r="K122" s="85"/>
@@ -5580,20 +5523,20 @@
     <row r="124" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A124" s="29"/>
       <c r="B124" s="30"/>
-      <c r="C124" s="111" t="s">
+      <c r="C124" s="137" t="s">
         <v>205</v>
       </c>
-      <c r="D124" s="116" t="s">
+      <c r="D124" s="142" t="s">
         <v>166</v>
       </c>
       <c r="E124" s="99" t="s">
         <v>167</v>
       </c>
-      <c r="F124" s="113">
+      <c r="F124" s="139">
         <v>0</v>
       </c>
-      <c r="G124" s="124"/>
-      <c r="H124" s="126" t="s">
+      <c r="G124" s="150"/>
+      <c r="H124" s="152" t="s">
         <v>14</v>
       </c>
       <c r="I124" s="17"/>
@@ -5610,14 +5553,14 @@
     <row r="125" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A125" s="29"/>
       <c r="B125" s="30"/>
-      <c r="C125" s="111"/>
-      <c r="D125" s="116"/>
+      <c r="C125" s="137"/>
+      <c r="D125" s="142"/>
       <c r="E125" s="99" t="s">
         <v>168</v>
       </c>
-      <c r="F125" s="114"/>
-      <c r="G125" s="125"/>
-      <c r="H125" s="126"/>
+      <c r="F125" s="140"/>
+      <c r="G125" s="151"/>
+      <c r="H125" s="152"/>
       <c r="I125" s="17"/>
       <c r="J125" s="17"/>
       <c r="K125" s="85"/>
@@ -5632,14 +5575,14 @@
     <row r="126" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A126" s="29"/>
       <c r="B126" s="30"/>
-      <c r="C126" s="111"/>
+      <c r="C126" s="137"/>
       <c r="D126" s="96" t="s">
         <v>169</v>
       </c>
       <c r="E126" s="99" t="s">
         <v>170</v>
       </c>
-      <c r="F126" s="114"/>
+      <c r="F126" s="140"/>
       <c r="G126" s="100"/>
       <c r="H126" s="98" t="s">
         <v>14</v>
@@ -5658,14 +5601,14 @@
     <row r="127" spans="1:18" s="7" customFormat="1" ht="25.5" customHeight="1">
       <c r="A127" s="29"/>
       <c r="B127" s="30"/>
-      <c r="C127" s="111"/>
+      <c r="C127" s="137"/>
       <c r="D127" s="96" t="s">
         <v>171</v>
       </c>
       <c r="E127" s="99" t="s">
         <v>172</v>
       </c>
-      <c r="F127" s="114"/>
+      <c r="F127" s="140"/>
       <c r="G127" s="100"/>
       <c r="H127" s="98" t="s">
         <v>14</v>
@@ -5684,14 +5627,14 @@
     <row r="128" spans="1:18" s="7" customFormat="1" ht="36.75" customHeight="1">
       <c r="A128" s="29"/>
       <c r="B128" s="30"/>
-      <c r="C128" s="111"/>
+      <c r="C128" s="137"/>
       <c r="D128" s="96" t="s">
         <v>176</v>
       </c>
       <c r="E128" s="99" t="s">
         <v>173</v>
       </c>
-      <c r="F128" s="114"/>
+      <c r="F128" s="140"/>
       <c r="G128" s="100"/>
       <c r="H128" s="98" t="s">
         <v>14</v>
@@ -5710,16 +5653,16 @@
     <row r="129" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A129" s="29"/>
       <c r="B129" s="30"/>
-      <c r="C129" s="111"/>
-      <c r="D129" s="116" t="s">
+      <c r="C129" s="137"/>
+      <c r="D129" s="142" t="s">
         <v>2</v>
       </c>
       <c r="E129" s="99" t="s">
         <v>174</v>
       </c>
-      <c r="F129" s="114"/>
-      <c r="G129" s="124"/>
-      <c r="H129" s="126" t="s">
+      <c r="F129" s="140"/>
+      <c r="G129" s="150"/>
+      <c r="H129" s="152" t="s">
         <v>14</v>
       </c>
       <c r="I129" s="17"/>
@@ -5736,14 +5679,14 @@
     <row r="130" spans="1:18" s="7" customFormat="1" ht="24.75" customHeight="1">
       <c r="A130" s="29"/>
       <c r="B130" s="30"/>
-      <c r="C130" s="111"/>
-      <c r="D130" s="116"/>
+      <c r="C130" s="137"/>
+      <c r="D130" s="142"/>
       <c r="E130" s="99" t="s">
         <v>175</v>
       </c>
-      <c r="F130" s="123"/>
-      <c r="G130" s="125"/>
-      <c r="H130" s="126"/>
+      <c r="F130" s="149"/>
+      <c r="G130" s="151"/>
+      <c r="H130" s="152"/>
       <c r="I130" s="17"/>
       <c r="J130" s="17"/>
       <c r="K130" s="85"/>
@@ -5822,20 +5765,20 @@
     <row r="134" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A134" s="29"/>
       <c r="B134" s="30"/>
-      <c r="C134" s="111" t="s">
+      <c r="C134" s="137" t="s">
         <v>209</v>
       </c>
-      <c r="D134" s="116" t="s">
+      <c r="D134" s="142" t="s">
         <v>178</v>
       </c>
       <c r="E134" s="99" t="s">
         <v>179</v>
       </c>
-      <c r="F134" s="113">
+      <c r="F134" s="139">
         <v>0</v>
       </c>
-      <c r="G134" s="124"/>
-      <c r="H134" s="126" t="s">
+      <c r="G134" s="150"/>
+      <c r="H134" s="152" t="s">
         <v>14</v>
       </c>
       <c r="I134" s="17"/>
@@ -5852,14 +5795,14 @@
     <row r="135" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A135" s="29"/>
       <c r="B135" s="30"/>
-      <c r="C135" s="111"/>
-      <c r="D135" s="116"/>
+      <c r="C135" s="137"/>
+      <c r="D135" s="142"/>
       <c r="E135" s="99" t="s">
         <v>180</v>
       </c>
-      <c r="F135" s="114"/>
-      <c r="G135" s="125"/>
-      <c r="H135" s="126"/>
+      <c r="F135" s="140"/>
+      <c r="G135" s="151"/>
+      <c r="H135" s="152"/>
       <c r="I135" s="17"/>
       <c r="J135" s="17"/>
       <c r="K135" s="85"/>
@@ -5874,14 +5817,14 @@
     <row r="136" spans="1:18" s="7" customFormat="1" ht="36" customHeight="1">
       <c r="A136" s="29"/>
       <c r="B136" s="30"/>
-      <c r="C136" s="111"/>
+      <c r="C136" s="137"/>
       <c r="D136" s="96" t="s">
         <v>188</v>
       </c>
       <c r="E136" s="99" t="s">
         <v>181</v>
       </c>
-      <c r="F136" s="114"/>
+      <c r="F136" s="140"/>
       <c r="G136" s="97" t="s">
         <v>14</v>
       </c>
@@ -5900,18 +5843,18 @@
     <row r="137" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A137" s="29"/>
       <c r="B137" s="30"/>
-      <c r="C137" s="111"/>
-      <c r="D137" s="116" t="s">
+      <c r="C137" s="137"/>
+      <c r="D137" s="142" t="s">
         <v>182</v>
       </c>
       <c r="E137" s="99" t="s">
         <v>183</v>
       </c>
-      <c r="F137" s="114"/>
-      <c r="G137" s="118" t="s">
+      <c r="F137" s="140"/>
+      <c r="G137" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="H137" s="120"/>
+      <c r="H137" s="146"/>
       <c r="I137" s="18"/>
       <c r="J137" s="18"/>
       <c r="K137" s="86"/>
@@ -5926,14 +5869,14 @@
     <row r="138" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A138" s="29"/>
       <c r="B138" s="30"/>
-      <c r="C138" s="111"/>
-      <c r="D138" s="116"/>
+      <c r="C138" s="137"/>
+      <c r="D138" s="142"/>
       <c r="E138" s="99" t="s">
         <v>184</v>
       </c>
-      <c r="F138" s="114"/>
-      <c r="G138" s="118"/>
-      <c r="H138" s="121"/>
+      <c r="F138" s="140"/>
+      <c r="G138" s="144"/>
+      <c r="H138" s="147"/>
       <c r="I138" s="18"/>
       <c r="J138" s="18"/>
       <c r="K138" s="86"/>
@@ -5948,14 +5891,14 @@
     <row r="139" spans="1:18" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A139" s="29"/>
       <c r="B139" s="30"/>
-      <c r="C139" s="111"/>
-      <c r="D139" s="116"/>
+      <c r="C139" s="137"/>
+      <c r="D139" s="142"/>
       <c r="E139" s="99" t="s">
         <v>185</v>
       </c>
-      <c r="F139" s="114"/>
-      <c r="G139" s="118"/>
-      <c r="H139" s="121"/>
+      <c r="F139" s="140"/>
+      <c r="G139" s="144"/>
+      <c r="H139" s="147"/>
       <c r="I139" s="18"/>
       <c r="J139" s="18"/>
       <c r="K139" s="86"/>
@@ -5970,14 +5913,14 @@
     <row r="140" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A140" s="29"/>
       <c r="B140" s="30"/>
-      <c r="C140" s="111"/>
-      <c r="D140" s="116"/>
+      <c r="C140" s="137"/>
+      <c r="D140" s="142"/>
       <c r="E140" s="99" t="s">
         <v>186</v>
       </c>
-      <c r="F140" s="114"/>
-      <c r="G140" s="118"/>
-      <c r="H140" s="121"/>
+      <c r="F140" s="140"/>
+      <c r="G140" s="144"/>
+      <c r="H140" s="147"/>
       <c r="I140" s="18"/>
       <c r="J140" s="18"/>
       <c r="K140" s="86"/>
@@ -5992,14 +5935,14 @@
     <row r="141" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A141" s="29"/>
       <c r="B141" s="30"/>
-      <c r="C141" s="111"/>
-      <c r="D141" s="116"/>
+      <c r="C141" s="137"/>
+      <c r="D141" s="142"/>
       <c r="E141" s="99" t="s">
         <v>187</v>
       </c>
-      <c r="F141" s="123"/>
-      <c r="G141" s="118"/>
-      <c r="H141" s="127"/>
+      <c r="F141" s="149"/>
+      <c r="G141" s="144"/>
+      <c r="H141" s="153"/>
       <c r="I141" s="18"/>
       <c r="J141" s="18"/>
       <c r="K141" s="86"/>
@@ -6036,7 +5979,7 @@
     <row r="143" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A143" s="29"/>
       <c r="B143" s="30"/>
-      <c r="C143" s="111" t="s">
+      <c r="C143" s="137" t="s">
         <v>206</v>
       </c>
       <c r="D143" s="96" t="s">
@@ -6045,7 +5988,7 @@
       <c r="E143" s="99" t="s">
         <v>191</v>
       </c>
-      <c r="F143" s="113">
+      <c r="F143" s="139">
         <v>0</v>
       </c>
       <c r="G143" s="97" t="s">
@@ -6066,18 +6009,18 @@
     <row r="144" spans="1:18" s="7" customFormat="1" ht="24" customHeight="1">
       <c r="A144" s="29"/>
       <c r="B144" s="30"/>
-      <c r="C144" s="111"/>
-      <c r="D144" s="116" t="s">
+      <c r="C144" s="137"/>
+      <c r="D144" s="142" t="s">
         <v>192</v>
       </c>
       <c r="E144" s="99" t="s">
         <v>193</v>
       </c>
-      <c r="F144" s="114"/>
-      <c r="G144" s="118" t="s">
+      <c r="F144" s="140"/>
+      <c r="G144" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="H144" s="120"/>
+      <c r="H144" s="146"/>
       <c r="I144" s="18"/>
       <c r="J144" s="18"/>
       <c r="K144" s="86"/>
@@ -6092,14 +6035,14 @@
     <row r="145" spans="1:18" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A145" s="29"/>
       <c r="B145" s="30"/>
-      <c r="C145" s="111"/>
-      <c r="D145" s="116"/>
+      <c r="C145" s="137"/>
+      <c r="D145" s="142"/>
       <c r="E145" s="99" t="s">
         <v>194</v>
       </c>
-      <c r="F145" s="114"/>
-      <c r="G145" s="118"/>
-      <c r="H145" s="121"/>
+      <c r="F145" s="140"/>
+      <c r="G145" s="144"/>
+      <c r="H145" s="147"/>
       <c r="I145" s="18"/>
       <c r="J145" s="18"/>
       <c r="K145" s="86"/>
@@ -6114,14 +6057,14 @@
     <row r="146" spans="1:18" s="7" customFormat="1" ht="12">
       <c r="A146" s="29"/>
       <c r="B146" s="30"/>
-      <c r="C146" s="111"/>
-      <c r="D146" s="116"/>
+      <c r="C146" s="137"/>
+      <c r="D146" s="142"/>
       <c r="E146" s="99" t="s">
         <v>195</v>
       </c>
-      <c r="F146" s="114"/>
-      <c r="G146" s="118"/>
-      <c r="H146" s="121"/>
+      <c r="F146" s="140"/>
+      <c r="G146" s="144"/>
+      <c r="H146" s="147"/>
       <c r="I146" s="18"/>
       <c r="J146" s="18"/>
       <c r="K146" s="86"/>
@@ -6136,14 +6079,14 @@
     <row r="147" spans="1:18" s="7" customFormat="1" ht="24.75" customHeight="1" thickBot="1">
       <c r="A147" s="52"/>
       <c r="B147" s="53"/>
-      <c r="C147" s="112"/>
-      <c r="D147" s="117"/>
+      <c r="C147" s="138"/>
+      <c r="D147" s="143"/>
       <c r="E147" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="F147" s="115"/>
-      <c r="G147" s="119"/>
-      <c r="H147" s="122"/>
+      <c r="F147" s="141"/>
+      <c r="G147" s="145"/>
+      <c r="H147" s="148"/>
       <c r="I147" s="18"/>
       <c r="J147" s="18"/>
       <c r="K147" s="90"/>
@@ -6439,15 +6382,9 @@
     <mergeCell ref="G129:G130"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="J10:Q147">
-    <cfRule type="expression" dxfId="3" priority="45">
-      <formula>J10="C"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="46">
-      <formula>J10="B"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="47">
-      <formula>J10="A"</formula>
+  <conditionalFormatting sqref="K10:M147 O10:Q147">
+    <cfRule type="expression" dxfId="0" priority="47">
+      <formula>K10&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.19" bottom="0.19" header="0.21" footer="0.19"/>
@@ -6467,7 +6404,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="I1" sqref="I1:R1048576"/>
       <selection pane="bottomLeft" activeCell="B1" sqref="B1:AL12"/>
-      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12.75"/>
@@ -6489,47 +6426,49 @@
     <row r="2" spans="1:11" ht="12.75" customHeight="1">
       <c r="A2" s="71"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="104" t="s">
+      <c r="C2" s="130" t="s">
         <v>207</v>
       </c>
-      <c r="D2" s="108" t="s">
+      <c r="D2" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="108"/>
-      <c r="F2" s="109"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="135"/>
       <c r="G2" s="67"/>
-      <c r="H2" s="110" t="s">
+      <c r="H2" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="108"/>
-      <c r="J2" s="109"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="135"/>
       <c r="K2" s="19"/>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1">
       <c r="A3" s="71"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="105"/>
+      <c r="C3" s="131"/>
       <c r="D3" s="65">
+        <f>'Progression - Programme'!K3</f>
         <v>1</v>
       </c>
       <c r="E3" s="55">
-        <f>D3+1</f>
+        <f>'Progression - Programme'!L3</f>
         <v>2</v>
       </c>
       <c r="F3" s="56">
-        <f>E3+1</f>
+        <f>'Progression - Programme'!M3</f>
         <v>3</v>
       </c>
       <c r="G3" s="68"/>
       <c r="H3" s="69">
+        <f>'Progression - Programme'!O3</f>
         <v>1</v>
       </c>
       <c r="I3" s="55">
-        <f>H3+1</f>
+        <f>'Progression - Programme'!P3</f>
         <v>2</v>
       </c>
       <c r="J3" s="56">
-        <f>I3+1</f>
+        <f>'Progression - Programme'!Q3</f>
         <v>3</v>
       </c>
       <c r="K3" s="20"/>
@@ -6539,7 +6478,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="105"/>
+      <c r="C4" s="131"/>
       <c r="D4" s="66">
         <f>'Progression - Programme'!K4</f>
         <v>0</v>
@@ -6568,7 +6507,7 @@
       <c r="K4" s="20"/>
     </row>
     <row r="5" spans="1:11" s="7" customFormat="1" ht="39" customHeight="1">
-      <c r="A5" s="139" t="s">
+      <c r="A5" s="104" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="64"/>
@@ -6603,7 +6542,7 @@
       <c r="K5" s="23"/>
     </row>
     <row r="6" spans="1:11" s="7" customFormat="1" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A6" s="164" t="s">
+      <c r="A6" s="107" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="35"/>
@@ -6638,210 +6577,210 @@
       <c r="K6" s="25"/>
     </row>
     <row r="7" spans="1:11" ht="6.75" customHeight="1" thickBot="1">
-      <c r="A7" s="162"/>
-      <c r="B7" s="163"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="163"/>
-      <c r="H7" s="163"/>
-      <c r="I7" s="163"/>
-      <c r="J7" s="163"/>
+      <c r="A7" s="105"/>
+      <c r="B7" s="106"/>
+      <c r="C7" s="106"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="106"/>
+      <c r="F7" s="106"/>
+      <c r="G7" s="106"/>
+      <c r="H7" s="106"/>
+      <c r="I7" s="106"/>
+      <c r="J7" s="106"/>
     </row>
     <row r="8" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A8" s="165"/>
-      <c r="B8" s="167"/>
-      <c r="C8" s="167"/>
-      <c r="D8" s="142"/>
-      <c r="E8" s="143"/>
-      <c r="F8" s="144"/>
-      <c r="G8" s="168"/>
-      <c r="H8" s="166"/>
-      <c r="I8" s="143"/>
-      <c r="J8" s="144"/>
+      <c r="A8" s="127"/>
+      <c r="B8" s="108"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="111"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="113"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="126"/>
+      <c r="I8" s="112"/>
+      <c r="J8" s="113"/>
     </row>
     <row r="9" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A9" s="148"/>
-      <c r="B9" s="167"/>
-      <c r="C9" s="167"/>
-      <c r="D9" s="149"/>
-      <c r="E9" s="150"/>
-      <c r="F9" s="151"/>
-      <c r="G9" s="168"/>
-      <c r="H9" s="152"/>
-      <c r="I9" s="150"/>
-      <c r="J9" s="151"/>
+      <c r="A9" s="128"/>
+      <c r="B9" s="108"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="115"/>
+      <c r="F9" s="116"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="120"/>
+      <c r="I9" s="115"/>
+      <c r="J9" s="116"/>
     </row>
     <row r="10" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A10" s="141"/>
-      <c r="B10" s="167"/>
-      <c r="C10" s="167"/>
-      <c r="D10" s="145"/>
-      <c r="E10" s="146"/>
-      <c r="F10" s="147"/>
-      <c r="G10" s="168"/>
-      <c r="H10" s="145"/>
-      <c r="I10" s="146"/>
-      <c r="J10" s="147"/>
+      <c r="A10" s="129"/>
+      <c r="B10" s="108"/>
+      <c r="C10" s="108"/>
+      <c r="D10" s="117"/>
+      <c r="E10" s="118"/>
+      <c r="F10" s="119"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="117"/>
+      <c r="I10" s="118"/>
+      <c r="J10" s="119"/>
     </row>
     <row r="11" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A11" s="148"/>
-      <c r="B11" s="167"/>
-      <c r="C11" s="167"/>
-      <c r="D11" s="152"/>
-      <c r="E11" s="150"/>
-      <c r="F11" s="151"/>
-      <c r="G11" s="168"/>
-      <c r="H11" s="152"/>
-      <c r="I11" s="150"/>
-      <c r="J11" s="151"/>
+      <c r="A11" s="128"/>
+      <c r="B11" s="108"/>
+      <c r="C11" s="108"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="115"/>
+      <c r="F11" s="116"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="120"/>
+      <c r="I11" s="115"/>
+      <c r="J11" s="116"/>
     </row>
     <row r="12" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A12" s="141"/>
-      <c r="B12" s="167"/>
-      <c r="C12" s="167"/>
-      <c r="D12" s="145"/>
-      <c r="E12" s="146"/>
-      <c r="F12" s="147"/>
-      <c r="G12" s="168"/>
-      <c r="H12" s="145"/>
-      <c r="I12" s="146"/>
-      <c r="J12" s="147"/>
+      <c r="A12" s="129"/>
+      <c r="B12" s="108"/>
+      <c r="C12" s="108"/>
+      <c r="D12" s="117"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="119"/>
+      <c r="G12" s="109"/>
+      <c r="H12" s="117"/>
+      <c r="I12" s="118"/>
+      <c r="J12" s="119"/>
     </row>
     <row r="13" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A13" s="148"/>
-      <c r="B13" s="167"/>
-      <c r="C13" s="167"/>
-      <c r="D13" s="153"/>
-      <c r="E13" s="150"/>
-      <c r="F13" s="151"/>
-      <c r="G13" s="168"/>
-      <c r="H13" s="152"/>
-      <c r="I13" s="150"/>
-      <c r="J13" s="151"/>
+      <c r="A13" s="128"/>
+      <c r="B13" s="108"/>
+      <c r="C13" s="108"/>
+      <c r="D13" s="121"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="116"/>
+      <c r="G13" s="109"/>
+      <c r="H13" s="120"/>
+      <c r="I13" s="115"/>
+      <c r="J13" s="116"/>
     </row>
     <row r="14" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A14" s="141"/>
-      <c r="B14" s="167"/>
-      <c r="C14" s="167"/>
-      <c r="D14" s="154"/>
-      <c r="E14" s="146"/>
-      <c r="F14" s="147"/>
-      <c r="G14" s="168"/>
-      <c r="H14" s="145"/>
-      <c r="I14" s="146"/>
-      <c r="J14" s="147"/>
+      <c r="A14" s="129"/>
+      <c r="B14" s="108"/>
+      <c r="C14" s="108"/>
+      <c r="D14" s="122"/>
+      <c r="E14" s="118"/>
+      <c r="F14" s="119"/>
+      <c r="G14" s="109"/>
+      <c r="H14" s="117"/>
+      <c r="I14" s="118"/>
+      <c r="J14" s="119"/>
     </row>
     <row r="15" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A15" s="148"/>
-      <c r="B15" s="167"/>
-      <c r="C15" s="167"/>
-      <c r="D15" s="152"/>
-      <c r="E15" s="150"/>
-      <c r="F15" s="151"/>
-      <c r="G15" s="168"/>
-      <c r="H15" s="152"/>
-      <c r="I15" s="150"/>
-      <c r="J15" s="151"/>
+      <c r="A15" s="128"/>
+      <c r="B15" s="108"/>
+      <c r="C15" s="108"/>
+      <c r="D15" s="120"/>
+      <c r="E15" s="115"/>
+      <c r="F15" s="116"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="120"/>
+      <c r="I15" s="115"/>
+      <c r="J15" s="116"/>
     </row>
     <row r="16" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A16" s="141"/>
-      <c r="B16" s="167"/>
-      <c r="C16" s="167"/>
-      <c r="D16" s="145"/>
-      <c r="E16" s="146"/>
-      <c r="F16" s="147"/>
-      <c r="G16" s="168"/>
-      <c r="H16" s="145"/>
-      <c r="I16" s="146"/>
-      <c r="J16" s="147"/>
+      <c r="A16" s="129"/>
+      <c r="B16" s="108"/>
+      <c r="C16" s="108"/>
+      <c r="D16" s="117"/>
+      <c r="E16" s="118"/>
+      <c r="F16" s="119"/>
+      <c r="G16" s="109"/>
+      <c r="H16" s="117"/>
+      <c r="I16" s="118"/>
+      <c r="J16" s="119"/>
     </row>
     <row r="17" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A17" s="148"/>
-      <c r="B17" s="167"/>
-      <c r="C17" s="167"/>
-      <c r="D17" s="152"/>
-      <c r="E17" s="150"/>
-      <c r="F17" s="151"/>
-      <c r="G17" s="168"/>
-      <c r="H17" s="152"/>
-      <c r="I17" s="150"/>
-      <c r="J17" s="151"/>
+      <c r="A17" s="128"/>
+      <c r="B17" s="108"/>
+      <c r="C17" s="108"/>
+      <c r="D17" s="120"/>
+      <c r="E17" s="115"/>
+      <c r="F17" s="116"/>
+      <c r="G17" s="109"/>
+      <c r="H17" s="120"/>
+      <c r="I17" s="115"/>
+      <c r="J17" s="116"/>
     </row>
     <row r="18" spans="1:11" s="94" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A18" s="155"/>
+      <c r="A18" s="129"/>
       <c r="B18" s="93"/>
       <c r="C18" s="93"/>
-      <c r="D18" s="156"/>
-      <c r="E18" s="157"/>
-      <c r="F18" s="158"/>
-      <c r="G18" s="169"/>
-      <c r="H18" s="156"/>
-      <c r="I18" s="157"/>
-      <c r="J18" s="158"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="118"/>
+      <c r="F18" s="119"/>
+      <c r="G18" s="110"/>
+      <c r="H18" s="117"/>
+      <c r="I18" s="118"/>
+      <c r="J18" s="119"/>
       <c r="K18" s="93"/>
     </row>
     <row r="19" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A19" s="148"/>
-      <c r="B19" s="167"/>
-      <c r="C19" s="167"/>
-      <c r="D19" s="153"/>
-      <c r="E19" s="150"/>
-      <c r="F19" s="151"/>
-      <c r="G19" s="168"/>
-      <c r="H19" s="152"/>
-      <c r="I19" s="150"/>
-      <c r="J19" s="151"/>
+      <c r="A19" s="128"/>
+      <c r="B19" s="108"/>
+      <c r="C19" s="108"/>
+      <c r="D19" s="121"/>
+      <c r="E19" s="115"/>
+      <c r="F19" s="116"/>
+      <c r="G19" s="109"/>
+      <c r="H19" s="120"/>
+      <c r="I19" s="115"/>
+      <c r="J19" s="116"/>
     </row>
     <row r="20" spans="1:11" s="94" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A20" s="155"/>
+      <c r="A20" s="129"/>
       <c r="B20" s="93"/>
       <c r="C20" s="93"/>
-      <c r="D20" s="156"/>
-      <c r="E20" s="157"/>
-      <c r="F20" s="158"/>
-      <c r="G20" s="169"/>
-      <c r="H20" s="156"/>
-      <c r="I20" s="157"/>
-      <c r="J20" s="158"/>
+      <c r="D20" s="117"/>
+      <c r="E20" s="118"/>
+      <c r="F20" s="119"/>
+      <c r="G20" s="110"/>
+      <c r="H20" s="117"/>
+      <c r="I20" s="118"/>
+      <c r="J20" s="119"/>
       <c r="K20" s="93"/>
     </row>
     <row r="21" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A21" s="148"/>
-      <c r="B21" s="167"/>
-      <c r="C21" s="167"/>
-      <c r="D21" s="152"/>
-      <c r="E21" s="150"/>
-      <c r="F21" s="151"/>
-      <c r="G21" s="168"/>
-      <c r="H21" s="152"/>
-      <c r="I21" s="150"/>
-      <c r="J21" s="151"/>
+      <c r="A21" s="128"/>
+      <c r="B21" s="108"/>
+      <c r="C21" s="108"/>
+      <c r="D21" s="120"/>
+      <c r="E21" s="115"/>
+      <c r="F21" s="116"/>
+      <c r="G21" s="109"/>
+      <c r="H21" s="120"/>
+      <c r="I21" s="115"/>
+      <c r="J21" s="116"/>
     </row>
     <row r="22" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A22" s="141"/>
-      <c r="B22" s="167"/>
-      <c r="C22" s="167"/>
-      <c r="D22" s="145"/>
-      <c r="E22" s="146"/>
-      <c r="F22" s="147"/>
-      <c r="G22" s="168"/>
-      <c r="H22" s="145"/>
-      <c r="I22" s="146"/>
-      <c r="J22" s="147"/>
+      <c r="A22" s="129"/>
+      <c r="B22" s="108"/>
+      <c r="C22" s="108"/>
+      <c r="D22" s="117"/>
+      <c r="E22" s="118"/>
+      <c r="F22" s="119"/>
+      <c r="G22" s="109"/>
+      <c r="H22" s="117"/>
+      <c r="I22" s="118"/>
+      <c r="J22" s="119"/>
     </row>
     <row r="23" spans="1:11" ht="32.25" customHeight="1" thickBot="1">
-      <c r="A23" s="140"/>
-      <c r="B23" s="167"/>
-      <c r="C23" s="167"/>
-      <c r="D23" s="159"/>
-      <c r="E23" s="160"/>
-      <c r="F23" s="161"/>
-      <c r="G23" s="168"/>
-      <c r="H23" s="159"/>
-      <c r="I23" s="160"/>
-      <c r="J23" s="161"/>
+      <c r="A23" s="107"/>
+      <c r="B23" s="108"/>
+      <c r="C23" s="108"/>
+      <c r="D23" s="123"/>
+      <c r="E23" s="124"/>
+      <c r="F23" s="125"/>
+      <c r="G23" s="109"/>
+      <c r="H23" s="123"/>
+      <c r="I23" s="124"/>
+      <c r="J23" s="125"/>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" deleteRows="0"/>
@@ -6850,11 +6789,6 @@
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="H2:J2"/>
   </mergeCells>
-  <conditionalFormatting sqref="F8:J23">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="52">
-      <formula>LEN(TRIM(F8))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.31" right="0.33" top="0.46" bottom="0.4" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="8" scale="35" orientation="portrait" horizontalDpi="4000" verticalDpi="4000" r:id="rId1"/>
 </worksheet>

</xml_diff>